<commit_message>
Added test code to the experments.py file and ran the first half of the first function
</commit_message>
<xml_diff>
--- a/data/results/raw_parameter_search/untrained_testing.xlsx
+++ b/data/results/raw_parameter_search/untrained_testing.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -50,7 +50,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -66,6 +65,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -411,34 +478,34 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1567131.938338502</v>
+        <v>1567115.623891188</v>
       </c>
       <c r="D2" t="n">
-        <v>1567050.454892668</v>
+        <v>1567138.46577982</v>
       </c>
       <c r="E2" t="n">
-        <v>1566741.3866912</v>
+        <v>1567030.788621371</v>
       </c>
       <c r="F2" t="n">
-        <v>1567077.42715084</v>
+        <v>1566926.162664846</v>
       </c>
       <c r="G2" t="n">
-        <v>1567095.831889566</v>
+        <v>1567207.703912765</v>
       </c>
       <c r="H2" t="n">
-        <v>1567173.997895742</v>
+        <v>1567253.086686487</v>
       </c>
       <c r="I2" t="n">
-        <v>1566915.726579338</v>
+        <v>1567028.905865692</v>
       </c>
       <c r="J2" t="n">
-        <v>1567124.853668956</v>
+        <v>1567165.431763784</v>
       </c>
       <c r="K2" t="n">
-        <v>1566739.778949379</v>
+        <v>1567337.728605261</v>
       </c>
       <c r="L2" t="n">
-        <v>1567087.736775672</v>
+        <v>1567233.742292779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>